<commit_message>
continue working on report
</commit_message>
<xml_diff>
--- a/CW2/Task4/Output.xlsx
+++ b/CW2/Task4/Output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke Waller\Documents\GitHub\Aint308\CW2\Task4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB06207-1D0A-417C-AF7B-4C2AE396CE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F704096C-303B-42FB-A2BB-D127443DE8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-2190" windowWidth="18240" windowHeight="28440" xr2:uid="{53A2A339-F438-4517-BA05-2E2D95F4DDE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{53A2A339-F438-4517-BA05-2E2D95F4DDE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Average Value</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">Distance x Disparity </t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
@@ -82,11 +85,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,7 +636,557 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Percentage Error over</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Distance - 10618407</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.27845348866899822"/>
+          <c:y val="1.7410226520298909E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$33:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$33:$B$45</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-5.53</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-4.95</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-3.91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-3.06</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B511-4BC6-80DD-FD809F24715A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1936582399"/>
+        <c:axId val="1936581567"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1936582399"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="150"/>
+          <c:min val="30"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Distance (cm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1936581567"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1936581567"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Percentage Error (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1936582399"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1188,6 +1742,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1221,6 +2291,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C469CEC9-B7C2-3E34-5302-76895B5193B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1526,10 +2632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC420AD-1219-4EC0-91D5-137D476D538F}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,8 +2837,191 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>30</v>
+      </c>
+      <c r="B33" s="2">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>40</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2.17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>50</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>60</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>70</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>80</v>
+      </c>
+      <c r="B38" s="2">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>90</v>
+      </c>
+      <c r="B39" s="2">
+        <v>3.24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>100</v>
+      </c>
+      <c r="B40" s="2">
+        <v>2.23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>110</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>120</v>
+      </c>
+      <c r="B42" s="2">
+        <v>-5.53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>130</v>
+      </c>
+      <c r="B43" s="2">
+        <v>-4.95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>140</v>
+      </c>
+      <c r="B44" s="2">
+        <v>-3.91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>150</v>
+      </c>
+      <c r="B45" s="2">
+        <v>-3.06</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{A7ED2EA8-65E7-4CE0-90AA-C8BCA13E426B}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!B33:B33</xm:f>
+              <xm:sqref>A33</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B34:B34</xm:f>
+              <xm:sqref>A34</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B35:B35</xm:f>
+              <xm:sqref>A35</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B36:B36</xm:f>
+              <xm:sqref>A36</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B37:B37</xm:f>
+              <xm:sqref>A37</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B38:B38</xm:f>
+              <xm:sqref>A38</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B39:B39</xm:f>
+              <xm:sqref>A39</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B40:B40</xm:f>
+              <xm:sqref>A40</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B41:B41</xm:f>
+              <xm:sqref>A41</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B42:B42</xm:f>
+              <xm:sqref>A42</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B43:B43</xm:f>
+              <xm:sqref>A43</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B44:B44</xm:f>
+              <xm:sqref>A44</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B45:B45</xm:f>
+              <xm:sqref>A45</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>